<commit_message>
updated corrs and novelty scoring
</commit_message>
<xml_diff>
--- a/novelty_scoring/autdata_test_novelty_combined.xlsx
+++ b/novelty_scoring/autdata_test_novelty_combined.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jhec8\Documents\Northwestern_SROP\AUT-Scoring\novelty_scoring\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{965897C5-AAAF-4F82-B440-7058C6A3AFDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0751D1A8-E995-4552-BBCD-1E48810F5BAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23820" yWindow="4245" windowWidth="21570" windowHeight="11835" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23160" yWindow="4260" windowWidth="21570" windowHeight="11835" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cup" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1614" uniqueCount="486">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1615" uniqueCount="486">
   <si>
     <t>id</t>
   </si>
@@ -1913,8 +1913,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S78"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D78" sqref="D78"/>
+    <sheetView topLeftCell="A57" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C63" sqref="C63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7194,8 +7194,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:E85"/>
   <sheetViews>
-    <sheetView topLeftCell="A69" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="D86" sqref="D86"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8641,9 +8641,9 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:H76"/>
+  <dimension ref="A1:L76"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
@@ -8652,7 +8652,7 @@
     <col min="3" max="3" width="39.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -8669,7 +8669,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>92</v>
       </c>
@@ -8686,7 +8686,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>92</v>
       </c>
@@ -8703,7 +8703,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -8720,7 +8720,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -8737,7 +8737,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -8754,7 +8754,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -8771,7 +8771,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>171</v>
       </c>
@@ -8788,7 +8788,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>171</v>
       </c>
@@ -8804,8 +8804,11 @@
       <c r="E9">
         <v>2</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="L9" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>171</v>
       </c>
@@ -8822,7 +8825,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>171</v>
       </c>
@@ -8839,7 +8842,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>171</v>
       </c>
@@ -8856,7 +8859,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>7</v>
       </c>
@@ -8873,7 +8876,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>7</v>
       </c>
@@ -8890,7 +8893,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>7</v>
       </c>
@@ -8907,7 +8910,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>8</v>
       </c>

</xml_diff>